<commit_message>
Set all scripts to run under "run_parameters"
</commit_message>
<xml_diff>
--- a/data/run_parameters.xlsx
+++ b/data/run_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkim\Dropbox\CLF\Research projects\2024-02 antibiotic footprints model\antibiotic_footprints\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750CAE45-3973-4941-8F49-E0134A2F89A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36F8146-B048-4734-8F52-F405E07EDE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="19890" windowHeight="11880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="26760" windowHeight="14520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="108">
   <si>
     <t>parameter</t>
   </si>
@@ -1744,8 +1744,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D37" sqref="D3:D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1793,6 +1793,9 @@
       <c r="C3" t="s">
         <v>21</v>
       </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
       <c r="E3" t="s">
         <v>41</v>
       </c>
@@ -1807,6 +1810,9 @@
       <c r="C4" t="s">
         <v>21</v>
       </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
       <c r="F4" t="s">
         <v>47</v>
       </c>
@@ -1821,6 +1827,9 @@
       <c r="C5" t="s">
         <v>21</v>
       </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
       <c r="E5" t="s">
         <v>52</v>
       </c>
@@ -1835,6 +1844,9 @@
       <c r="C6" t="s">
         <v>21</v>
       </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
       <c r="E6" t="s">
         <v>51</v>
       </c>
@@ -1852,6 +1864,9 @@
       <c r="C7" t="s">
         <v>21</v>
       </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
       <c r="F7" t="s">
         <v>48</v>
       </c>
@@ -1866,6 +1881,9 @@
       <c r="C8" t="s">
         <v>21</v>
       </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1877,6 +1895,9 @@
       <c r="C9" t="s">
         <v>21</v>
       </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1888,6 +1909,9 @@
       <c r="C10" t="s">
         <v>21</v>
       </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1899,6 +1923,9 @@
       <c r="C11" t="s">
         <v>21</v>
       </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
       <c r="F11" t="s">
         <v>45</v>
       </c>
@@ -1913,6 +1940,9 @@
       <c r="C12" t="s">
         <v>21</v>
       </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1924,6 +1954,9 @@
       <c r="C13" t="s">
         <v>21</v>
       </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
       <c r="F13" t="s">
         <v>71</v>
       </c>
@@ -1938,6 +1971,9 @@
       <c r="C14" t="s">
         <v>21</v>
       </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
       <c r="E14" t="s">
         <v>105</v>
       </c>
@@ -1955,6 +1991,9 @@
       <c r="C15" t="s">
         <v>21</v>
       </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1966,6 +2005,9 @@
       <c r="C16" t="s">
         <v>21</v>
       </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
       <c r="E16" t="s">
         <v>105</v>
       </c>
@@ -1983,6 +2025,9 @@
       <c r="C17" t="s">
         <v>21</v>
       </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
       <c r="E17" t="s">
         <v>68</v>
       </c>
@@ -2000,6 +2045,9 @@
       <c r="C18" t="s">
         <v>21</v>
       </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
       <c r="E18" t="s">
         <v>104</v>
       </c>
@@ -2014,6 +2062,9 @@
       <c r="C19" t="s">
         <v>21</v>
       </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -2025,6 +2076,9 @@
       <c r="C20" t="s">
         <v>21</v>
       </c>
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -2036,6 +2090,9 @@
       <c r="C21" t="s">
         <v>21</v>
       </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
       <c r="E21" t="s">
         <v>105</v>
       </c>
@@ -2050,6 +2107,9 @@
       <c r="C22" t="s">
         <v>21</v>
       </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -2061,6 +2121,9 @@
       <c r="C23" t="s">
         <v>23</v>
       </c>
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
       <c r="F23" t="s">
         <v>19</v>
       </c>
@@ -2075,6 +2138,9 @@
       <c r="C24" t="s">
         <v>22</v>
       </c>
+      <c r="D24" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -2086,6 +2152,9 @@
       <c r="C25" t="s">
         <v>22</v>
       </c>
+      <c r="D25" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -2097,6 +2166,9 @@
       <c r="C26" t="s">
         <v>22</v>
       </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -2108,6 +2180,9 @@
       <c r="C27" t="s">
         <v>22</v>
       </c>
+      <c r="D27" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -2119,6 +2194,9 @@
       <c r="C28" t="s">
         <v>22</v>
       </c>
+      <c r="D28" t="s">
+        <v>2</v>
+      </c>
       <c r="E28" t="s">
         <v>58</v>
       </c>
@@ -2133,6 +2211,9 @@
       <c r="C29" t="s">
         <v>22</v>
       </c>
+      <c r="D29" t="s">
+        <v>2</v>
+      </c>
       <c r="E29" t="s">
         <v>64</v>
       </c>
@@ -2147,6 +2228,9 @@
       <c r="C30" t="s">
         <v>22</v>
       </c>
+      <c r="D30" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -2158,6 +2242,9 @@
       <c r="C31" t="s">
         <v>22</v>
       </c>
+      <c r="D31" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -2169,6 +2256,9 @@
       <c r="C32" t="s">
         <v>22</v>
       </c>
+      <c r="D32" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -2180,6 +2270,9 @@
       <c r="C33" t="s">
         <v>22</v>
       </c>
+      <c r="D33" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -2191,6 +2284,9 @@
       <c r="C34" t="s">
         <v>22</v>
       </c>
+      <c r="D34" t="s">
+        <v>2</v>
+      </c>
       <c r="E34" t="s">
         <v>107</v>
       </c>
@@ -2205,6 +2301,9 @@
       <c r="C35" t="s">
         <v>22</v>
       </c>
+      <c r="D35" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -2216,6 +2315,9 @@
       <c r="C36" t="s">
         <v>22</v>
       </c>
+      <c r="D36" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -2226,6 +2328,9 @@
       </c>
       <c r="C37" t="s">
         <v>22</v>
+      </c>
+      <c r="D37" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Corrections to figures 4 and 5 y-axis labels; additional details for Pearson tests
</commit_message>
<xml_diff>
--- a/data/run_parameters.xlsx
+++ b/data/run_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkim\Dropbox\CLF\Research projects\2024-02 antibiotic footprints model\antibiotic_footprints\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36F8146-B048-4734-8F52-F405E07EDE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99BFD33-1359-40DC-9820-B923A11F44B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="26760" windowHeight="14520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="855" yWindow="2415" windowWidth="19890" windowHeight="11520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="6" r:id="rId1"/>
@@ -1745,7 +1745,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D37" sqref="D3:D37"/>
+      <selection activeCell="D38" sqref="D3:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>